<commit_message>
Added standard PZ books
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Steam\project-zomboid-trading-technology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4921E65E-8BBE-46C0-A8E2-EA19B2EB9D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87C6868-69F5-4E68-9AA1-2F9AB586ECE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5530FF74-5E2D-4318-B60A-E243DAB36AB7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5530FF74-5E2D-4318-B60A-E243DAB36AB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="663">
   <si>
     <t>HCBook</t>
   </si>
@@ -1771,6 +1771,261 @@
   </si>
   <si>
     <t>Столбец8</t>
+  </si>
+  <si>
+    <t>RadioMag1</t>
+  </si>
+  <si>
+    <t>RadioMag2</t>
+  </si>
+  <si>
+    <t>RadioMag3</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>ProjectZomboid</t>
+  </si>
+  <si>
+    <t>BookTrapping1</t>
+  </si>
+  <si>
+    <t>BookTrapping2</t>
+  </si>
+  <si>
+    <t>BookTrapping3</t>
+  </si>
+  <si>
+    <t>BookTrapping4</t>
+  </si>
+  <si>
+    <t>BookTrapping5</t>
+  </si>
+  <si>
+    <t>BookFishing1</t>
+  </si>
+  <si>
+    <t>BookFishing2</t>
+  </si>
+  <si>
+    <t>BookFishing3</t>
+  </si>
+  <si>
+    <t>BookFishing4</t>
+  </si>
+  <si>
+    <t>BookFishing5</t>
+  </si>
+  <si>
+    <t>BookCarpentry1</t>
+  </si>
+  <si>
+    <t>BookCarpentry2</t>
+  </si>
+  <si>
+    <t>BookCarpentry3</t>
+  </si>
+  <si>
+    <t>BookCarpentry4</t>
+  </si>
+  <si>
+    <t>BookCarpentry5</t>
+  </si>
+  <si>
+    <t>BookMechanic1</t>
+  </si>
+  <si>
+    <t>BookMechanic2</t>
+  </si>
+  <si>
+    <t>BookMechanic3</t>
+  </si>
+  <si>
+    <t>BookMechanic4</t>
+  </si>
+  <si>
+    <t>BookMechanic5</t>
+  </si>
+  <si>
+    <t>BookFirstAid1</t>
+  </si>
+  <si>
+    <t>BookFirstAid2</t>
+  </si>
+  <si>
+    <t>BookFirstAid3</t>
+  </si>
+  <si>
+    <t>BookFirstAid4</t>
+  </si>
+  <si>
+    <t>BookFirstAid5</t>
+  </si>
+  <si>
+    <t>BookBlacksmith1</t>
+  </si>
+  <si>
+    <t>BookBlacksmith2</t>
+  </si>
+  <si>
+    <t>BookBlacksmith3</t>
+  </si>
+  <si>
+    <t>BookBlacksmith4</t>
+  </si>
+  <si>
+    <t>BookBlacksmith5</t>
+  </si>
+  <si>
+    <t>BookMetalWelding1</t>
+  </si>
+  <si>
+    <t>BookMetalWelding2</t>
+  </si>
+  <si>
+    <t>BookMetalWelding3</t>
+  </si>
+  <si>
+    <t>BookMetalWelding4</t>
+  </si>
+  <si>
+    <t>BookMetalWelding5</t>
+  </si>
+  <si>
+    <t>BookElectrician1</t>
+  </si>
+  <si>
+    <t>BookElectrician2</t>
+  </si>
+  <si>
+    <t>BookElectrician3</t>
+  </si>
+  <si>
+    <t>BookElectrician4</t>
+  </si>
+  <si>
+    <t>BookElectrician5</t>
+  </si>
+  <si>
+    <t>BookCooking1</t>
+  </si>
+  <si>
+    <t>BookCooking2</t>
+  </si>
+  <si>
+    <t>BookCooking3</t>
+  </si>
+  <si>
+    <t>BookCooking4</t>
+  </si>
+  <si>
+    <t>BookCooking5</t>
+  </si>
+  <si>
+    <t>BookFarming1</t>
+  </si>
+  <si>
+    <t>BookFarming2</t>
+  </si>
+  <si>
+    <t>BookFarming3</t>
+  </si>
+  <si>
+    <t>BookFarming4</t>
+  </si>
+  <si>
+    <t>BookFarming5</t>
+  </si>
+  <si>
+    <t>BookForaging1</t>
+  </si>
+  <si>
+    <t>BookForaging2</t>
+  </si>
+  <si>
+    <t>BookForaging3</t>
+  </si>
+  <si>
+    <t>BookForaging4</t>
+  </si>
+  <si>
+    <t>BookForaging5</t>
+  </si>
+  <si>
+    <t>BookTailoring1</t>
+  </si>
+  <si>
+    <t>BookTailoring2</t>
+  </si>
+  <si>
+    <t>BookTailoring3</t>
+  </si>
+  <si>
+    <t>BookTailoring4</t>
+  </si>
+  <si>
+    <t>BookTailoring5</t>
+  </si>
+  <si>
+    <t>MechanicMag1</t>
+  </si>
+  <si>
+    <t>MechanicMag2</t>
+  </si>
+  <si>
+    <t>MechanicMag3</t>
+  </si>
+  <si>
+    <t>FarmingMag1</t>
+  </si>
+  <si>
+    <t>FishingMag1</t>
+  </si>
+  <si>
+    <t>FishingMag2</t>
+  </si>
+  <si>
+    <t>HuntingMag1</t>
+  </si>
+  <si>
+    <t>HuntingMag2</t>
+  </si>
+  <si>
+    <t>HuntingMag3</t>
+  </si>
+  <si>
+    <t>HerbalistMag</t>
+  </si>
+  <si>
+    <t>CookingMag1</t>
+  </si>
+  <si>
+    <t>CookingMag2</t>
+  </si>
+  <si>
+    <t>ElectronicsMag1</t>
+  </si>
+  <si>
+    <t>ElectronicsMag2</t>
+  </si>
+  <si>
+    <t>ElectronicsMag3</t>
+  </si>
+  <si>
+    <t>ElectronicsMag4</t>
+  </si>
+  <si>
+    <t>ElectronicsMag5</t>
+  </si>
+  <si>
+    <t>EngineerMagazine1</t>
+  </si>
+  <si>
+    <t>EngineerMagazine2</t>
+  </si>
+  <si>
+    <t>Doodle</t>
   </si>
 </sst>
 </file>
@@ -1829,10 +2084,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2218,15 +2474,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F13742-AA5C-4FE6-84A6-26AB79E74EAE}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
@@ -3865,6 +4121,96 @@
         <f t="shared" si="1"/>
         <v>PornoMag1/PornoMag1b/PornoMag2/PornoMag2b/PornoMag3/PornoMag3b/PornoMag4/PornoMag4b/PornoMag5/PornoMag5b/PornoMag6/PornoMag6b</v>
       </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>582</v>
+      </c>
+      <c r="B118" t="s">
+        <v>398</v>
+      </c>
+      <c r="C118" t="s">
+        <v>254</v>
+      </c>
+      <c r="D118" t="str">
+        <f>C118</f>
+        <v>Book</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>582</v>
+      </c>
+      <c r="B120" t="s">
+        <v>398</v>
+      </c>
+      <c r="C120" t="s">
+        <v>261</v>
+      </c>
+      <c r="D120" t="str">
+        <f>C120</f>
+        <v>Magazine</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>582</v>
+      </c>
+      <c r="B121" t="s">
+        <v>398</v>
+      </c>
+      <c r="C121" t="s">
+        <v>259</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" ref="D121" si="2">D120&amp;"/"&amp;C121</f>
+        <v>Magazine/HottieZ</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>582</v>
+      </c>
+      <c r="B122" t="s">
+        <v>398</v>
+      </c>
+      <c r="C122" t="s">
+        <v>262</v>
+      </c>
+      <c r="D122" t="str">
+        <f>D121&amp;"/"&amp;C122</f>
+        <v>Magazine/HottieZ/Newspaper</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>582</v>
+      </c>
+      <c r="B123" t="s">
+        <v>398</v>
+      </c>
+      <c r="C123" t="s">
+        <v>256</v>
+      </c>
+      <c r="D123" t="str">
+        <f>D122&amp;"/"&amp;C123</f>
+        <v>Magazine/HottieZ/Newspaper/ComicBook</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3877,15 +4223,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC077BC-C7FC-45EA-9A6A-E0F8EB815209}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
@@ -4205,20 +4551,81 @@
         <v>HCBookcover/HCBookmark</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>582</v>
+      </c>
+      <c r="B26" t="s">
+        <v>398</v>
+      </c>
+      <c r="C26" t="s">
+        <v>263</v>
+      </c>
+      <c r="D26" t="str">
+        <f>C26</f>
+        <v>Notebook</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>582</v>
+      </c>
+      <c r="B27" t="s">
+        <v>398</v>
+      </c>
+      <c r="C27" t="s">
+        <v>662</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" ref="D27:D29" si="1">D26&amp;"/"&amp;C27</f>
+        <v>Notebook/Doodle</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>582</v>
+      </c>
+      <c r="B28" t="s">
+        <v>398</v>
+      </c>
+      <c r="C28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>Notebook/Doodle/Journal</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>582</v>
+      </c>
+      <c r="B29" t="s">
+        <v>398</v>
+      </c>
+      <c r="C29" t="s">
+        <v>264</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>Notebook/Doodle/Journal/SheetPaper2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBB719C-480D-4BE2-B1C1-76D3B3A3AC08}">
-  <dimension ref="A1:D335"/>
+  <dimension ref="A1:D367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D335" sqref="D335"/>
+    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
+      <selection activeCell="D367" sqref="D367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8758,6 +9165,456 @@
         <v>MakeWeapon</v>
       </c>
     </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>582</v>
+      </c>
+      <c r="B337" t="s">
+        <v>581</v>
+      </c>
+      <c r="C337" t="s">
+        <v>578</v>
+      </c>
+      <c r="D337" t="str">
+        <f>C337</f>
+        <v>RadioMag1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>582</v>
+      </c>
+      <c r="B338" t="s">
+        <v>581</v>
+      </c>
+      <c r="C338" t="s">
+        <v>579</v>
+      </c>
+      <c r="D338" t="str">
+        <f t="shared" ref="D338:D339" si="6">D337&amp;"/"&amp;C338</f>
+        <v>RadioMag1/RadioMag2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>582</v>
+      </c>
+      <c r="B339" t="s">
+        <v>581</v>
+      </c>
+      <c r="C339" t="s">
+        <v>580</v>
+      </c>
+      <c r="D339" t="str">
+        <f t="shared" si="6"/>
+        <v>RadioMag1/RadioMag2/RadioMag3</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>582</v>
+      </c>
+      <c r="B341" t="s">
+        <v>398</v>
+      </c>
+      <c r="C341" t="s">
+        <v>643</v>
+      </c>
+      <c r="D341" t="str">
+        <f>C341</f>
+        <v>MechanicMag1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>582</v>
+      </c>
+      <c r="B342" t="s">
+        <v>398</v>
+      </c>
+      <c r="C342" t="s">
+        <v>644</v>
+      </c>
+      <c r="D342" t="str">
+        <f t="shared" ref="D342:D367" si="7">D341&amp;"/"&amp;C342</f>
+        <v>MechanicMag1/MechanicMag2</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>582</v>
+      </c>
+      <c r="B343" t="s">
+        <v>398</v>
+      </c>
+      <c r="C343" t="s">
+        <v>645</v>
+      </c>
+      <c r="D343" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>582</v>
+      </c>
+      <c r="B344" t="s">
+        <v>398</v>
+      </c>
+      <c r="C344" t="s">
+        <v>646</v>
+      </c>
+      <c r="D344" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>582</v>
+      </c>
+      <c r="B345" t="s">
+        <v>398</v>
+      </c>
+      <c r="C345" t="s">
+        <v>647</v>
+      </c>
+      <c r="D345" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>582</v>
+      </c>
+      <c r="B346" t="s">
+        <v>398</v>
+      </c>
+      <c r="C346" t="s">
+        <v>648</v>
+      </c>
+      <c r="D346" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>582</v>
+      </c>
+      <c r="B347" t="s">
+        <v>398</v>
+      </c>
+      <c r="C347" t="s">
+        <v>649</v>
+      </c>
+      <c r="D347" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>582</v>
+      </c>
+      <c r="B348" t="s">
+        <v>398</v>
+      </c>
+      <c r="C348" t="s">
+        <v>650</v>
+      </c>
+      <c r="D348" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>582</v>
+      </c>
+      <c r="B349" t="s">
+        <v>398</v>
+      </c>
+      <c r="C349" t="s">
+        <v>651</v>
+      </c>
+      <c r="D349" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>582</v>
+      </c>
+      <c r="B350" t="s">
+        <v>398</v>
+      </c>
+      <c r="C350" t="s">
+        <v>652</v>
+      </c>
+      <c r="D350" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>582</v>
+      </c>
+      <c r="B351" t="s">
+        <v>398</v>
+      </c>
+      <c r="C351" t="s">
+        <v>267</v>
+      </c>
+      <c r="D351" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>582</v>
+      </c>
+      <c r="B352" t="s">
+        <v>398</v>
+      </c>
+      <c r="C352" t="s">
+        <v>268</v>
+      </c>
+      <c r="D352" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>582</v>
+      </c>
+      <c r="B353" t="s">
+        <v>398</v>
+      </c>
+      <c r="C353" t="s">
+        <v>269</v>
+      </c>
+      <c r="D353" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>582</v>
+      </c>
+      <c r="B354" t="s">
+        <v>398</v>
+      </c>
+      <c r="C354" t="s">
+        <v>220</v>
+      </c>
+      <c r="D354" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>582</v>
+      </c>
+      <c r="B355" t="s">
+        <v>398</v>
+      </c>
+      <c r="C355" t="s">
+        <v>226</v>
+      </c>
+      <c r="D355" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>582</v>
+      </c>
+      <c r="B356" t="s">
+        <v>398</v>
+      </c>
+      <c r="C356" t="s">
+        <v>227</v>
+      </c>
+      <c r="D356" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>582</v>
+      </c>
+      <c r="B357" t="s">
+        <v>398</v>
+      </c>
+      <c r="C357" t="s">
+        <v>228</v>
+      </c>
+      <c r="D357" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>582</v>
+      </c>
+      <c r="B358" t="s">
+        <v>398</v>
+      </c>
+      <c r="C358" t="s">
+        <v>229</v>
+      </c>
+      <c r="D358" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>582</v>
+      </c>
+      <c r="B359" t="s">
+        <v>398</v>
+      </c>
+      <c r="C359" t="s">
+        <v>653</v>
+      </c>
+      <c r="D359" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>582</v>
+      </c>
+      <c r="B360" t="s">
+        <v>398</v>
+      </c>
+      <c r="C360" t="s">
+        <v>654</v>
+      </c>
+      <c r="D360" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>582</v>
+      </c>
+      <c r="B361" t="s">
+        <v>398</v>
+      </c>
+      <c r="C361" t="s">
+        <v>655</v>
+      </c>
+      <c r="D361" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2/ElectronicsMag1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>582</v>
+      </c>
+      <c r="B362" t="s">
+        <v>398</v>
+      </c>
+      <c r="C362" t="s">
+        <v>656</v>
+      </c>
+      <c r="D362" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2/ElectronicsMag1/ElectronicsMag2</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>582</v>
+      </c>
+      <c r="B363" t="s">
+        <v>398</v>
+      </c>
+      <c r="C363" t="s">
+        <v>657</v>
+      </c>
+      <c r="D363" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2/ElectronicsMag1/ElectronicsMag2/ElectronicsMag3</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>582</v>
+      </c>
+      <c r="B364" t="s">
+        <v>398</v>
+      </c>
+      <c r="C364" t="s">
+        <v>658</v>
+      </c>
+      <c r="D364" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2/ElectronicsMag1/ElectronicsMag2/ElectronicsMag3/ElectronicsMag4</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>582</v>
+      </c>
+      <c r="B365" t="s">
+        <v>398</v>
+      </c>
+      <c r="C365" t="s">
+        <v>659</v>
+      </c>
+      <c r="D365" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2/ElectronicsMag1/ElectronicsMag2/ElectronicsMag3/ElectronicsMag4/ElectronicsMag5</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>582</v>
+      </c>
+      <c r="B366" t="s">
+        <v>398</v>
+      </c>
+      <c r="C366" t="s">
+        <v>660</v>
+      </c>
+      <c r="D366" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2/ElectronicsMag1/ElectronicsMag2/ElectronicsMag3/ElectronicsMag4/ElectronicsMag5/EngineerMagazine1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>582</v>
+      </c>
+      <c r="B367" t="s">
+        <v>398</v>
+      </c>
+      <c r="C367" t="s">
+        <v>661</v>
+      </c>
+      <c r="D367" t="str">
+        <f t="shared" si="7"/>
+        <v>MechanicMag1/MechanicMag2/MechanicMag3/FarmingMag1/FishingMag1/FishingMag2/HuntingMag1/HuntingMag2/HuntingMag3/HerbalistMag/MetalworkMag1/MetalworkMag2/MetalworkMag3/MetalworkMag4/SmithingMag1/SmithingMag2/SmithingMag3/SmithingMag4/CookingMag1/CookingMag2/ElectronicsMag1/ElectronicsMag2/ElectronicsMag3/ElectronicsMag4/ElectronicsMag5/EngineerMagazine1/EngineerMagazine2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8768,10 +9625,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F68E0F5-EB59-4E31-81B5-F9C8EA325DE6}">
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:L6"/>
+    <sheetView topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="L170" sqref="L170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8854,7 +9711,7 @@
         <v>BookMaintenance1</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I2:I3" si="1">D3</f>
+        <f t="shared" ref="I3" si="1">D3</f>
         <v>BookMaintenance2</v>
       </c>
     </row>
@@ -8877,7 +9734,7 @@
         <v>BookMaintenance2</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ref="J2:J4" si="3">E4</f>
+        <f t="shared" ref="J4" si="3">E4</f>
         <v>BookMaintenance3</v>
       </c>
     </row>
@@ -8904,7 +9761,7 @@
         <v>BookMaintenance3</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K2:K5" si="5">F5</f>
+        <f t="shared" ref="K5" si="5">F5</f>
         <v>BookMaintenance4</v>
       </c>
     </row>
@@ -8931,11 +9788,11 @@
         <v>BookMaintenance3</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" ref="K6:L7" si="6">IF(ISBLANK(F6),K5,K5&amp;"/"&amp;F6)</f>
+        <f t="shared" ref="K6" si="6">IF(ISBLANK(F6),K5,K5&amp;"/"&amp;F6)</f>
         <v>BookMaintenance4</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" ref="L2:L6" si="7">G6</f>
+        <f t="shared" ref="L6" si="7">G6</f>
         <v>BookMaintenance5</v>
       </c>
     </row>
@@ -8969,7 +9826,7 @@
         <v>BookSleeping1</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9:I10" si="9">D9</f>
+        <f t="shared" ref="I9" si="9">D9</f>
         <v>BookSleeping2</v>
       </c>
     </row>
@@ -8992,7 +9849,7 @@
         <v>BookSleeping2</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" ref="J10:J12" si="10">E10</f>
+        <f t="shared" ref="J10" si="10">E10</f>
         <v>BookSleeping3</v>
       </c>
     </row>
@@ -9019,7 +9876,7 @@
         <v>BookSleeping3</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" ref="K11:K12" si="11">F11</f>
+        <f t="shared" ref="K11" si="11">F11</f>
         <v>BookSleeping4</v>
       </c>
     </row>
@@ -9050,7 +9907,7 @@
         <v>BookSleeping4</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" ref="L12:L13" si="12">G12</f>
+        <f t="shared" ref="L12" si="12">G12</f>
         <v>BookSleeping5</v>
       </c>
     </row>
@@ -9084,7 +9941,7 @@
         <v>BookSmithing1</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" ref="I15:I16" si="14">D15</f>
+        <f t="shared" ref="I15" si="14">D15</f>
         <v>BookSmithing2</v>
       </c>
     </row>
@@ -9107,7 +9964,7 @@
         <v>BookSmithing2</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" ref="J16:J18" si="15">E16</f>
+        <f t="shared" ref="J16" si="15">E16</f>
         <v>BookSmithing3</v>
       </c>
     </row>
@@ -9134,7 +9991,7 @@
         <v>BookSmithing3</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ref="K17:K18" si="16">F17</f>
+        <f t="shared" ref="K17" si="16">F17</f>
         <v>BookSmithing4</v>
       </c>
     </row>
@@ -9165,7 +10022,7 @@
         <v>BookSmithing4</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" ref="L18:L19" si="17">G18</f>
+        <f t="shared" ref="L18" si="17">G18</f>
         <v>BookSmithing5</v>
       </c>
     </row>
@@ -9199,7 +10056,7 @@
         <v>BookMasonry1</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" ref="I21:I22" si="19">D21</f>
+        <f t="shared" ref="I21" si="19">D21</f>
         <v>BookMasonry2</v>
       </c>
     </row>
@@ -9222,7 +10079,7 @@
         <v>BookMasonry2</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ref="J22:J24" si="20">E22</f>
+        <f t="shared" ref="J22" si="20">E22</f>
         <v>BookMasonry3</v>
       </c>
     </row>
@@ -9249,7 +10106,7 @@
         <v>BookMasonry3</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" ref="K23:K24" si="21">F23</f>
+        <f t="shared" ref="K23" si="21">F23</f>
         <v>BookMasonry4</v>
       </c>
     </row>
@@ -9333,7 +10190,7 @@
         <v>BookAiming1</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" ref="I29:I30" si="24">D29</f>
+        <f t="shared" ref="I29" si="24">D29</f>
         <v>BookAiming2</v>
       </c>
     </row>
@@ -9356,7 +10213,7 @@
         <v>BookAiming2</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" ref="J30:J32" si="25">E30</f>
+        <f t="shared" ref="J30" si="25">E30</f>
         <v>BookAiming3</v>
       </c>
     </row>
@@ -9383,7 +10240,7 @@
         <v>BookAiming3</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" ref="K31:K32" si="26">F31</f>
+        <f t="shared" ref="K31" si="26">F31</f>
         <v>BookAiming4</v>
       </c>
     </row>
@@ -9414,7 +10271,7 @@
         <v>BookAiming4</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" ref="L32:L33" si="27">G32</f>
+        <f t="shared" ref="L32" si="27">G32</f>
         <v>BookAiming5</v>
       </c>
     </row>
@@ -11308,7 +12165,7 @@
         <v>BookStrength1</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" ref="I95:I96" si="31">D95</f>
+        <f t="shared" ref="I95" si="31">D95</f>
         <v>BookStrength2</v>
       </c>
     </row>
@@ -11331,7 +12188,7 @@
         <v>BookStrength2</v>
       </c>
       <c r="J96" t="str">
-        <f t="shared" ref="J96:J98" si="32">E96</f>
+        <f t="shared" ref="J96" si="32">E96</f>
         <v>BookStrength3</v>
       </c>
     </row>
@@ -11358,7 +12215,7 @@
         <v>BookStrength3</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" ref="K97:K98" si="33">F97</f>
+        <f t="shared" ref="K97" si="33">F97</f>
         <v>BookStrength4</v>
       </c>
     </row>
@@ -11389,7 +12246,7 @@
         <v>BookStrength4</v>
       </c>
       <c r="L98" t="str">
-        <f t="shared" ref="L98:L104" si="34">G98</f>
+        <f t="shared" ref="L98" si="34">G98</f>
         <v>BookStrength5</v>
       </c>
     </row>
@@ -11420,7 +12277,7 @@
         <v>BookStrength4</v>
       </c>
       <c r="L99" t="str">
-        <f t="shared" ref="L99:L104" si="35">IF(ISBLANK(G99),L98,L98&amp;"/"&amp;G99)</f>
+        <f t="shared" ref="L99:L103" si="35">IF(ISBLANK(G99),L98,L98&amp;"/"&amp;G99)</f>
         <v>BookStrength5</v>
       </c>
     </row>
@@ -11578,7 +12435,7 @@
         <v>BookLockpicking1</v>
       </c>
       <c r="I106" t="str">
-        <f t="shared" ref="I106:I107" si="37">D106</f>
+        <f t="shared" ref="I106" si="37">D106</f>
         <v>BookLockpicking2</v>
       </c>
     </row>
@@ -11601,7 +12458,7 @@
         <v>BookLockpicking2</v>
       </c>
       <c r="J107" t="str">
-        <f t="shared" ref="J107:J109" si="38">E107</f>
+        <f t="shared" ref="J107" si="38">E107</f>
         <v>BookLockpicking3</v>
       </c>
     </row>
@@ -11628,7 +12485,7 @@
         <v>BookLockpicking3</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" ref="K108:K109" si="39">F108</f>
+        <f t="shared" ref="K108" si="39">F108</f>
         <v>BookLockpicking4</v>
       </c>
     </row>
@@ -11661,6 +12518,1826 @@
       <c r="L109" t="str">
         <f t="shared" ref="L109" si="40">G109</f>
         <v>BookLockpicking5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>582</v>
+      </c>
+      <c r="B111" t="s">
+        <v>398</v>
+      </c>
+      <c r="C111" t="s">
+        <v>583</v>
+      </c>
+      <c r="H111" t="str">
+        <f t="shared" ref="H111" si="41">C111</f>
+        <v>BookTrapping1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>582</v>
+      </c>
+      <c r="B112" t="s">
+        <v>398</v>
+      </c>
+      <c r="D112" t="s">
+        <v>584</v>
+      </c>
+      <c r="H112" t="str">
+        <f t="shared" ref="H112:H170" si="42">IF(ISBLANK(C112),H111,H111&amp;"/"&amp;C112)</f>
+        <v>BookTrapping1</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" ref="I112" si="43">D112</f>
+        <v>BookTrapping2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>582</v>
+      </c>
+      <c r="B113" t="s">
+        <v>398</v>
+      </c>
+      <c r="E113" t="s">
+        <v>585</v>
+      </c>
+      <c r="H113" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1</v>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" ref="I113:I170" si="44">IF(ISBLANK(D113),I112,I112&amp;"/"&amp;D113)</f>
+        <v>BookTrapping2</v>
+      </c>
+      <c r="J113" t="str">
+        <f t="shared" ref="J113" si="45">E113</f>
+        <v>BookTrapping3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>582</v>
+      </c>
+      <c r="B114" t="s">
+        <v>398</v>
+      </c>
+      <c r="F114" t="s">
+        <v>586</v>
+      </c>
+      <c r="H114" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1</v>
+      </c>
+      <c r="I114" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2</v>
+      </c>
+      <c r="J114" t="str">
+        <f t="shared" ref="J114:J170" si="46">IF(ISBLANK(E114),J113,J113&amp;"/"&amp;E114)</f>
+        <v>BookTrapping3</v>
+      </c>
+      <c r="K114" t="str">
+        <f t="shared" ref="K114" si="47">F114</f>
+        <v>BookTrapping4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>582</v>
+      </c>
+      <c r="B115" t="s">
+        <v>398</v>
+      </c>
+      <c r="G115" t="s">
+        <v>587</v>
+      </c>
+      <c r="H115" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1</v>
+      </c>
+      <c r="I115" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2</v>
+      </c>
+      <c r="J115" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3</v>
+      </c>
+      <c r="K115" t="str">
+        <f t="shared" ref="K115:L170" si="48">IF(ISBLANK(F115),K114,K114&amp;"/"&amp;F115)</f>
+        <v>BookTrapping4</v>
+      </c>
+      <c r="L115" t="str">
+        <f t="shared" ref="L115" si="49">G115</f>
+        <v>BookTrapping5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>582</v>
+      </c>
+      <c r="B116" t="s">
+        <v>398</v>
+      </c>
+      <c r="C116" t="s">
+        <v>588</v>
+      </c>
+      <c r="H116" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1</v>
+      </c>
+      <c r="I116" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2</v>
+      </c>
+      <c r="J116" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3</v>
+      </c>
+      <c r="K116" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4</v>
+      </c>
+      <c r="L116" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>582</v>
+      </c>
+      <c r="B117" t="s">
+        <v>398</v>
+      </c>
+      <c r="D117" t="s">
+        <v>589</v>
+      </c>
+      <c r="H117" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1</v>
+      </c>
+      <c r="I117" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2</v>
+      </c>
+      <c r="J117" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3</v>
+      </c>
+      <c r="K117" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4</v>
+      </c>
+      <c r="L117" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>582</v>
+      </c>
+      <c r="B118" t="s">
+        <v>398</v>
+      </c>
+      <c r="E118" t="s">
+        <v>590</v>
+      </c>
+      <c r="H118" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1</v>
+      </c>
+      <c r="I118" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2</v>
+      </c>
+      <c r="J118" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3</v>
+      </c>
+      <c r="K118" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4</v>
+      </c>
+      <c r="L118" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>582</v>
+      </c>
+      <c r="B119" t="s">
+        <v>398</v>
+      </c>
+      <c r="F119" t="s">
+        <v>591</v>
+      </c>
+      <c r="H119" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1</v>
+      </c>
+      <c r="I119" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2</v>
+      </c>
+      <c r="J119" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3</v>
+      </c>
+      <c r="K119" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4</v>
+      </c>
+      <c r="L119" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>582</v>
+      </c>
+      <c r="B120" t="s">
+        <v>398</v>
+      </c>
+      <c r="G120" t="s">
+        <v>592</v>
+      </c>
+      <c r="H120" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1</v>
+      </c>
+      <c r="I120" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2</v>
+      </c>
+      <c r="J120" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3</v>
+      </c>
+      <c r="K120" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4</v>
+      </c>
+      <c r="L120" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>582</v>
+      </c>
+      <c r="B121" t="s">
+        <v>398</v>
+      </c>
+      <c r="C121" t="s">
+        <v>593</v>
+      </c>
+      <c r="H121" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1</v>
+      </c>
+      <c r="I121" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2</v>
+      </c>
+      <c r="J121" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3</v>
+      </c>
+      <c r="K121" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4</v>
+      </c>
+      <c r="L121" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>582</v>
+      </c>
+      <c r="B122" t="s">
+        <v>398</v>
+      </c>
+      <c r="D122" t="s">
+        <v>594</v>
+      </c>
+      <c r="H122" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1</v>
+      </c>
+      <c r="I122" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2</v>
+      </c>
+      <c r="J122" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3</v>
+      </c>
+      <c r="K122" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4</v>
+      </c>
+      <c r="L122" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>582</v>
+      </c>
+      <c r="B123" t="s">
+        <v>398</v>
+      </c>
+      <c r="E123" t="s">
+        <v>595</v>
+      </c>
+      <c r="H123" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1</v>
+      </c>
+      <c r="I123" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2</v>
+      </c>
+      <c r="J123" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3</v>
+      </c>
+      <c r="K123" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4</v>
+      </c>
+      <c r="L123" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>582</v>
+      </c>
+      <c r="B124" t="s">
+        <v>398</v>
+      </c>
+      <c r="F124" t="s">
+        <v>596</v>
+      </c>
+      <c r="H124" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1</v>
+      </c>
+      <c r="I124" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2</v>
+      </c>
+      <c r="J124" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3</v>
+      </c>
+      <c r="K124" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4</v>
+      </c>
+      <c r="L124" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>582</v>
+      </c>
+      <c r="B125" t="s">
+        <v>398</v>
+      </c>
+      <c r="G125" t="s">
+        <v>597</v>
+      </c>
+      <c r="H125" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1</v>
+      </c>
+      <c r="I125" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2</v>
+      </c>
+      <c r="J125" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3</v>
+      </c>
+      <c r="K125" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4</v>
+      </c>
+      <c r="L125" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>582</v>
+      </c>
+      <c r="B126" t="s">
+        <v>398</v>
+      </c>
+      <c r="C126" t="s">
+        <v>598</v>
+      </c>
+      <c r="H126" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1</v>
+      </c>
+      <c r="I126" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2</v>
+      </c>
+      <c r="J126" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3</v>
+      </c>
+      <c r="K126" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4</v>
+      </c>
+      <c r="L126" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>582</v>
+      </c>
+      <c r="B127" t="s">
+        <v>398</v>
+      </c>
+      <c r="D127" t="s">
+        <v>599</v>
+      </c>
+      <c r="H127" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1</v>
+      </c>
+      <c r="I127" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2</v>
+      </c>
+      <c r="J127" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3</v>
+      </c>
+      <c r="K127" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4</v>
+      </c>
+      <c r="L127" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>582</v>
+      </c>
+      <c r="B128" t="s">
+        <v>398</v>
+      </c>
+      <c r="E128" t="s">
+        <v>600</v>
+      </c>
+      <c r="H128" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1</v>
+      </c>
+      <c r="I128" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2</v>
+      </c>
+      <c r="J128" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3</v>
+      </c>
+      <c r="K128" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4</v>
+      </c>
+      <c r="L128" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>582</v>
+      </c>
+      <c r="B129" t="s">
+        <v>398</v>
+      </c>
+      <c r="F129" t="s">
+        <v>601</v>
+      </c>
+      <c r="H129" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1</v>
+      </c>
+      <c r="I129" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2</v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3</v>
+      </c>
+      <c r="K129" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4</v>
+      </c>
+      <c r="L129" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>582</v>
+      </c>
+      <c r="B130" t="s">
+        <v>398</v>
+      </c>
+      <c r="G130" t="s">
+        <v>602</v>
+      </c>
+      <c r="H130" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1</v>
+      </c>
+      <c r="I130" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2</v>
+      </c>
+      <c r="J130" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3</v>
+      </c>
+      <c r="K130" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4</v>
+      </c>
+      <c r="L130" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>582</v>
+      </c>
+      <c r="B131" t="s">
+        <v>398</v>
+      </c>
+      <c r="C131" t="s">
+        <v>603</v>
+      </c>
+      <c r="H131" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2</v>
+      </c>
+      <c r="J131" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3</v>
+      </c>
+      <c r="K131" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4</v>
+      </c>
+      <c r="L131" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>582</v>
+      </c>
+      <c r="B132" t="s">
+        <v>398</v>
+      </c>
+      <c r="D132" t="s">
+        <v>604</v>
+      </c>
+      <c r="H132" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2</v>
+      </c>
+      <c r="J132" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3</v>
+      </c>
+      <c r="K132" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4</v>
+      </c>
+      <c r="L132" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>582</v>
+      </c>
+      <c r="B133" t="s">
+        <v>398</v>
+      </c>
+      <c r="E133" t="s">
+        <v>605</v>
+      </c>
+      <c r="H133" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2</v>
+      </c>
+      <c r="J133" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3</v>
+      </c>
+      <c r="K133" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4</v>
+      </c>
+      <c r="L133" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>582</v>
+      </c>
+      <c r="B134" t="s">
+        <v>398</v>
+      </c>
+      <c r="F134" t="s">
+        <v>606</v>
+      </c>
+      <c r="H134" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2</v>
+      </c>
+      <c r="J134" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3</v>
+      </c>
+      <c r="K134" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4</v>
+      </c>
+      <c r="L134" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>582</v>
+      </c>
+      <c r="B135" t="s">
+        <v>398</v>
+      </c>
+      <c r="G135" t="s">
+        <v>607</v>
+      </c>
+      <c r="H135" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2</v>
+      </c>
+      <c r="J135" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3</v>
+      </c>
+      <c r="K135" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4</v>
+      </c>
+      <c r="L135" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>582</v>
+      </c>
+      <c r="B136" t="s">
+        <v>398</v>
+      </c>
+      <c r="C136" t="s">
+        <v>608</v>
+      </c>
+      <c r="H136" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1</v>
+      </c>
+      <c r="I136" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2</v>
+      </c>
+      <c r="J136" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3</v>
+      </c>
+      <c r="K136" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4</v>
+      </c>
+      <c r="L136" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>582</v>
+      </c>
+      <c r="B137" t="s">
+        <v>398</v>
+      </c>
+      <c r="D137" t="s">
+        <v>609</v>
+      </c>
+      <c r="H137" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1</v>
+      </c>
+      <c r="I137" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2</v>
+      </c>
+      <c r="J137" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3</v>
+      </c>
+      <c r="K137" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4</v>
+      </c>
+      <c r="L137" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>582</v>
+      </c>
+      <c r="B138" t="s">
+        <v>398</v>
+      </c>
+      <c r="E138" t="s">
+        <v>610</v>
+      </c>
+      <c r="H138" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1</v>
+      </c>
+      <c r="I138" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2</v>
+      </c>
+      <c r="J138" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3</v>
+      </c>
+      <c r="K138" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4</v>
+      </c>
+      <c r="L138" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>582</v>
+      </c>
+      <c r="B139" t="s">
+        <v>398</v>
+      </c>
+      <c r="F139" t="s">
+        <v>611</v>
+      </c>
+      <c r="H139" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1</v>
+      </c>
+      <c r="I139" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2</v>
+      </c>
+      <c r="J139" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3</v>
+      </c>
+      <c r="K139" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4</v>
+      </c>
+      <c r="L139" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>582</v>
+      </c>
+      <c r="B140" t="s">
+        <v>398</v>
+      </c>
+      <c r="G140" t="s">
+        <v>612</v>
+      </c>
+      <c r="H140" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1</v>
+      </c>
+      <c r="I140" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2</v>
+      </c>
+      <c r="J140" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3</v>
+      </c>
+      <c r="K140" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4</v>
+      </c>
+      <c r="L140" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>582</v>
+      </c>
+      <c r="B141" t="s">
+        <v>398</v>
+      </c>
+      <c r="C141" t="s">
+        <v>613</v>
+      </c>
+      <c r="H141" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1</v>
+      </c>
+      <c r="I141" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2</v>
+      </c>
+      <c r="J141" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3</v>
+      </c>
+      <c r="K141" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4</v>
+      </c>
+      <c r="L141" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>582</v>
+      </c>
+      <c r="B142" t="s">
+        <v>398</v>
+      </c>
+      <c r="D142" t="s">
+        <v>614</v>
+      </c>
+      <c r="H142" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1</v>
+      </c>
+      <c r="I142" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2</v>
+      </c>
+      <c r="J142" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3</v>
+      </c>
+      <c r="K142" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4</v>
+      </c>
+      <c r="L142" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>582</v>
+      </c>
+      <c r="B143" t="s">
+        <v>398</v>
+      </c>
+      <c r="E143" t="s">
+        <v>615</v>
+      </c>
+      <c r="H143" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1</v>
+      </c>
+      <c r="I143" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2</v>
+      </c>
+      <c r="J143" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3</v>
+      </c>
+      <c r="K143" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4</v>
+      </c>
+      <c r="L143" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>582</v>
+      </c>
+      <c r="B144" t="s">
+        <v>398</v>
+      </c>
+      <c r="F144" t="s">
+        <v>616</v>
+      </c>
+      <c r="H144" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1</v>
+      </c>
+      <c r="I144" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2</v>
+      </c>
+      <c r="J144" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3</v>
+      </c>
+      <c r="K144" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4</v>
+      </c>
+      <c r="L144" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>582</v>
+      </c>
+      <c r="B145" t="s">
+        <v>398</v>
+      </c>
+      <c r="G145" t="s">
+        <v>617</v>
+      </c>
+      <c r="H145" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1</v>
+      </c>
+      <c r="I145" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2</v>
+      </c>
+      <c r="J145" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3</v>
+      </c>
+      <c r="K145" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4</v>
+      </c>
+      <c r="L145" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>582</v>
+      </c>
+      <c r="B146" t="s">
+        <v>398</v>
+      </c>
+      <c r="C146" t="s">
+        <v>618</v>
+      </c>
+      <c r="H146" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1</v>
+      </c>
+      <c r="I146" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2</v>
+      </c>
+      <c r="J146" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3</v>
+      </c>
+      <c r="K146" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4</v>
+      </c>
+      <c r="L146" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>582</v>
+      </c>
+      <c r="B147" t="s">
+        <v>398</v>
+      </c>
+      <c r="D147" t="s">
+        <v>619</v>
+      </c>
+      <c r="H147" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1</v>
+      </c>
+      <c r="I147" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2</v>
+      </c>
+      <c r="J147" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3</v>
+      </c>
+      <c r="K147" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4</v>
+      </c>
+      <c r="L147" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>582</v>
+      </c>
+      <c r="B148" t="s">
+        <v>398</v>
+      </c>
+      <c r="E148" t="s">
+        <v>620</v>
+      </c>
+      <c r="H148" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1</v>
+      </c>
+      <c r="I148" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2</v>
+      </c>
+      <c r="J148" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3</v>
+      </c>
+      <c r="K148" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4</v>
+      </c>
+      <c r="L148" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>582</v>
+      </c>
+      <c r="B149" t="s">
+        <v>398</v>
+      </c>
+      <c r="F149" t="s">
+        <v>621</v>
+      </c>
+      <c r="H149" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1</v>
+      </c>
+      <c r="I149" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2</v>
+      </c>
+      <c r="J149" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3</v>
+      </c>
+      <c r="K149" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4</v>
+      </c>
+      <c r="L149" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>582</v>
+      </c>
+      <c r="B150" t="s">
+        <v>398</v>
+      </c>
+      <c r="G150" t="s">
+        <v>622</v>
+      </c>
+      <c r="H150" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1</v>
+      </c>
+      <c r="I150" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2</v>
+      </c>
+      <c r="J150" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3</v>
+      </c>
+      <c r="K150" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4</v>
+      </c>
+      <c r="L150" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>582</v>
+      </c>
+      <c r="B151" t="s">
+        <v>398</v>
+      </c>
+      <c r="C151" t="s">
+        <v>623</v>
+      </c>
+      <c r="H151" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1</v>
+      </c>
+      <c r="I151" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2</v>
+      </c>
+      <c r="J151" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3</v>
+      </c>
+      <c r="K151" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4</v>
+      </c>
+      <c r="L151" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>582</v>
+      </c>
+      <c r="B152" t="s">
+        <v>398</v>
+      </c>
+      <c r="D152" t="s">
+        <v>624</v>
+      </c>
+      <c r="H152" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1</v>
+      </c>
+      <c r="I152" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2</v>
+      </c>
+      <c r="J152" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3</v>
+      </c>
+      <c r="K152" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4</v>
+      </c>
+      <c r="L152" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>582</v>
+      </c>
+      <c r="B153" t="s">
+        <v>398</v>
+      </c>
+      <c r="E153" t="s">
+        <v>625</v>
+      </c>
+      <c r="H153" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1</v>
+      </c>
+      <c r="I153" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2</v>
+      </c>
+      <c r="J153" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3</v>
+      </c>
+      <c r="K153" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4</v>
+      </c>
+      <c r="L153" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>582</v>
+      </c>
+      <c r="B154" t="s">
+        <v>398</v>
+      </c>
+      <c r="F154" t="s">
+        <v>626</v>
+      </c>
+      <c r="H154" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1</v>
+      </c>
+      <c r="I154" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2</v>
+      </c>
+      <c r="J154" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3</v>
+      </c>
+      <c r="K154" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4</v>
+      </c>
+      <c r="L154" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>582</v>
+      </c>
+      <c r="B155" t="s">
+        <v>398</v>
+      </c>
+      <c r="G155" t="s">
+        <v>627</v>
+      </c>
+      <c r="H155" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1</v>
+      </c>
+      <c r="I155" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2</v>
+      </c>
+      <c r="J155" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3</v>
+      </c>
+      <c r="K155" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4</v>
+      </c>
+      <c r="L155" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>582</v>
+      </c>
+      <c r="B156" t="s">
+        <v>398</v>
+      </c>
+      <c r="C156" t="s">
+        <v>628</v>
+      </c>
+      <c r="H156" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1</v>
+      </c>
+      <c r="I156" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2</v>
+      </c>
+      <c r="J156" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3</v>
+      </c>
+      <c r="K156" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4</v>
+      </c>
+      <c r="L156" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>582</v>
+      </c>
+      <c r="B157" t="s">
+        <v>398</v>
+      </c>
+      <c r="D157" t="s">
+        <v>629</v>
+      </c>
+      <c r="H157" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1</v>
+      </c>
+      <c r="I157" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2</v>
+      </c>
+      <c r="J157" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3</v>
+      </c>
+      <c r="K157" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4</v>
+      </c>
+      <c r="L157" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>582</v>
+      </c>
+      <c r="B158" t="s">
+        <v>398</v>
+      </c>
+      <c r="E158" t="s">
+        <v>630</v>
+      </c>
+      <c r="H158" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1</v>
+      </c>
+      <c r="I158" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2</v>
+      </c>
+      <c r="J158" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3</v>
+      </c>
+      <c r="K158" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4</v>
+      </c>
+      <c r="L158" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>582</v>
+      </c>
+      <c r="B159" t="s">
+        <v>398</v>
+      </c>
+      <c r="F159" t="s">
+        <v>631</v>
+      </c>
+      <c r="H159" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1</v>
+      </c>
+      <c r="I159" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2</v>
+      </c>
+      <c r="J159" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3</v>
+      </c>
+      <c r="K159" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4</v>
+      </c>
+      <c r="L159" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>582</v>
+      </c>
+      <c r="B160" t="s">
+        <v>398</v>
+      </c>
+      <c r="G160" t="s">
+        <v>632</v>
+      </c>
+      <c r="H160" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1</v>
+      </c>
+      <c r="I160" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2</v>
+      </c>
+      <c r="J160" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3</v>
+      </c>
+      <c r="K160" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4</v>
+      </c>
+      <c r="L160" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>582</v>
+      </c>
+      <c r="B161" t="s">
+        <v>398</v>
+      </c>
+      <c r="C161" t="s">
+        <v>633</v>
+      </c>
+      <c r="H161" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1</v>
+      </c>
+      <c r="I161" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2</v>
+      </c>
+      <c r="J161" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3</v>
+      </c>
+      <c r="K161" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4</v>
+      </c>
+      <c r="L161" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>582</v>
+      </c>
+      <c r="B162" t="s">
+        <v>398</v>
+      </c>
+      <c r="D162" t="s">
+        <v>634</v>
+      </c>
+      <c r="H162" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1</v>
+      </c>
+      <c r="I162" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2</v>
+      </c>
+      <c r="J162" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3</v>
+      </c>
+      <c r="K162" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4</v>
+      </c>
+      <c r="L162" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>582</v>
+      </c>
+      <c r="B163" t="s">
+        <v>398</v>
+      </c>
+      <c r="E163" t="s">
+        <v>635</v>
+      </c>
+      <c r="H163" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1</v>
+      </c>
+      <c r="I163" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2</v>
+      </c>
+      <c r="J163" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3</v>
+      </c>
+      <c r="K163" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4</v>
+      </c>
+      <c r="L163" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>582</v>
+      </c>
+      <c r="B164" t="s">
+        <v>398</v>
+      </c>
+      <c r="F164" t="s">
+        <v>636</v>
+      </c>
+      <c r="H164" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1</v>
+      </c>
+      <c r="I164" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2</v>
+      </c>
+      <c r="J164" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3</v>
+      </c>
+      <c r="K164" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4/BookForaging4</v>
+      </c>
+      <c r="L164" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>582</v>
+      </c>
+      <c r="B165" t="s">
+        <v>398</v>
+      </c>
+      <c r="G165" t="s">
+        <v>637</v>
+      </c>
+      <c r="H165" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1</v>
+      </c>
+      <c r="I165" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2</v>
+      </c>
+      <c r="J165" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3</v>
+      </c>
+      <c r="K165" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4/BookForaging4</v>
+      </c>
+      <c r="L165" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5/BookForaging5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>582</v>
+      </c>
+      <c r="B166" t="s">
+        <v>398</v>
+      </c>
+      <c r="C166" t="s">
+        <v>638</v>
+      </c>
+      <c r="H166" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1/BookTailoring1</v>
+      </c>
+      <c r="I166" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2</v>
+      </c>
+      <c r="J166" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3</v>
+      </c>
+      <c r="K166" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4/BookForaging4</v>
+      </c>
+      <c r="L166" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5/BookForaging5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>582</v>
+      </c>
+      <c r="B167" t="s">
+        <v>398</v>
+      </c>
+      <c r="D167" t="s">
+        <v>639</v>
+      </c>
+      <c r="H167" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1/BookTailoring1</v>
+      </c>
+      <c r="I167" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2/BookTailoring2</v>
+      </c>
+      <c r="J167" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3</v>
+      </c>
+      <c r="K167" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4/BookForaging4</v>
+      </c>
+      <c r="L167" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5/BookForaging5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>582</v>
+      </c>
+      <c r="B168" t="s">
+        <v>398</v>
+      </c>
+      <c r="E168" t="s">
+        <v>640</v>
+      </c>
+      <c r="H168" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1/BookTailoring1</v>
+      </c>
+      <c r="I168" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2/BookTailoring2</v>
+      </c>
+      <c r="J168" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3/BookTailoring3</v>
+      </c>
+      <c r="K168" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4/BookForaging4</v>
+      </c>
+      <c r="L168" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5/BookForaging5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>582</v>
+      </c>
+      <c r="B169" t="s">
+        <v>398</v>
+      </c>
+      <c r="F169" t="s">
+        <v>641</v>
+      </c>
+      <c r="H169" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1/BookTailoring1</v>
+      </c>
+      <c r="I169" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2/BookTailoring2</v>
+      </c>
+      <c r="J169" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3/BookTailoring3</v>
+      </c>
+      <c r="K169" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4/BookForaging4/BookTailoring4</v>
+      </c>
+      <c r="L169" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5/BookForaging5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>582</v>
+      </c>
+      <c r="B170" t="s">
+        <v>398</v>
+      </c>
+      <c r="G170" t="s">
+        <v>642</v>
+      </c>
+      <c r="H170" t="str">
+        <f t="shared" si="42"/>
+        <v>BookTrapping1/BookFishing1/BookCarpentry1/BookMechanic1/BookFirstAid1/BookBlacksmith1/BookMetalWelding1/BookElectrician1/BookCooking1/BookFarming1/BookForaging1/BookTailoring1</v>
+      </c>
+      <c r="I170" t="str">
+        <f t="shared" si="44"/>
+        <v>BookTrapping2/BookFishing2/BookCarpentry2/BookMechanic2/BookFirstAid2/BookBlacksmith2/BookMetalWelding2/BookElectrician2/BookCooking2/BookFarming2/BookForaging2/BookTailoring2</v>
+      </c>
+      <c r="J170" t="str">
+        <f t="shared" si="46"/>
+        <v>BookTrapping3/BookFishing3/BookCarpentry3/BookMechanic3/BookFirstAid3/BookBlacksmith3/BookMetalWelding3/BookElectrician3/BookCooking3/BookFarming3/BookForaging3/BookTailoring3</v>
+      </c>
+      <c r="K170" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping4/BookFishing4/BookCarpentry4/BookMechanic4/BookFirstAid4/BookBlacksmith4/BookMetalWelding4/BookElectrician4/BookCooking4/BookFarming4/BookForaging4/BookTailoring4</v>
+      </c>
+      <c r="L170" t="str">
+        <f t="shared" si="48"/>
+        <v>BookTrapping5/BookFishing5/BookCarpentry5/BookMechanic5/BookFirstAid5/BookBlacksmith5/BookMetalWelding5/BookElectrician5/BookCooking5/BookFarming5/BookForaging5/BookTailoring5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>